<commit_message>
feat: adicionadas novas opções de valores pré-definidos na cobertura retrátil, novas lógicas de cálculo no orçamento e novo campo 'Custo de Deslocamento' no pergolado
</commit_message>
<xml_diff>
--- a/resources/PROPOSTA  - COBERTURA RETRÁTIL.xlsx
+++ b/resources/PROPOSTA  - COBERTURA RETRÁTIL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\Gabriela\pdf_generator\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A29EC792-0193-4B76-A45D-1AC5E8BE1AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E29D1C5-5CD3-4066-B912-36D1080EA35C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>Nome:</t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t>40 dias úteis</t>
+  </si>
+  <si>
+    <t>[Valor Total Geral]</t>
   </si>
 </sst>
 </file>
@@ -1139,7 +1142,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="158">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="21" borderId="0" xfId="34" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1276,6 +1279,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="21" borderId="18" xfId="33" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="21" borderId="19" xfId="33" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="21" borderId="23" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2115,8 +2121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:P59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="89" zoomScaleNormal="89" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43:L43"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="89" zoomScaleNormal="89" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="M47" sqref="M47:N47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2161,18 +2167,18 @@
     </row>
     <row r="3" spans="2:16" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="14"/>
-      <c r="C3" s="128"/>
-      <c r="D3" s="128"/>
-      <c r="E3" s="128"/>
-      <c r="F3" s="128"/>
-      <c r="G3" s="128"/>
-      <c r="H3" s="128"/>
-      <c r="I3" s="128"/>
-      <c r="J3" s="128"/>
-      <c r="K3" s="128"/>
-      <c r="L3" s="128"/>
-      <c r="M3" s="128"/>
-      <c r="N3" s="128"/>
+      <c r="C3" s="129"/>
+      <c r="D3" s="129"/>
+      <c r="E3" s="129"/>
+      <c r="F3" s="129"/>
+      <c r="G3" s="129"/>
+      <c r="H3" s="129"/>
+      <c r="I3" s="129"/>
+      <c r="J3" s="129"/>
+      <c r="K3" s="129"/>
+      <c r="L3" s="129"/>
+      <c r="M3" s="129"/>
+      <c r="N3" s="129"/>
       <c r="O3" s="19"/>
     </row>
     <row r="4" spans="2:16" ht="4.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2204,15 +2210,15 @@
         <v>14</v>
       </c>
       <c r="G6" s="25"/>
-      <c r="H6" s="92" t="s">
+      <c r="H6" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="92"/>
-      <c r="J6" s="92"/>
-      <c r="K6" s="92"/>
-      <c r="L6" s="92"/>
-      <c r="M6" s="92"/>
-      <c r="N6" s="93"/>
+      <c r="I6" s="93"/>
+      <c r="J6" s="93"/>
+      <c r="K6" s="93"/>
+      <c r="L6" s="93"/>
+      <c r="M6" s="93"/>
+      <c r="N6" s="94"/>
       <c r="O6" s="7"/>
     </row>
     <row r="7" spans="2:16" ht="14.25" x14ac:dyDescent="0.2">
@@ -2222,15 +2228,15 @@
       <c r="E7" s="1"/>
       <c r="F7" s="25"/>
       <c r="G7" s="25"/>
-      <c r="H7" s="94" t="s">
+      <c r="H7" s="95" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="94"/>
-      <c r="J7" s="94"/>
-      <c r="K7" s="94"/>
-      <c r="L7" s="94"/>
-      <c r="M7" s="94"/>
-      <c r="N7" s="95"/>
+      <c r="I7" s="95"/>
+      <c r="J7" s="95"/>
+      <c r="K7" s="95"/>
+      <c r="L7" s="95"/>
+      <c r="M7" s="95"/>
+      <c r="N7" s="96"/>
       <c r="O7" s="28"/>
       <c r="P7" s="14"/>
     </row>
@@ -2241,15 +2247,15 @@
       <c r="E8" s="1"/>
       <c r="F8" s="26"/>
       <c r="G8" s="26"/>
-      <c r="H8" s="94" t="s">
+      <c r="H8" s="95" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="94"/>
-      <c r="J8" s="94"/>
-      <c r="K8" s="94"/>
-      <c r="L8" s="94"/>
-      <c r="M8" s="94"/>
-      <c r="N8" s="95"/>
+      <c r="I8" s="95"/>
+      <c r="J8" s="95"/>
+      <c r="K8" s="95"/>
+      <c r="L8" s="95"/>
+      <c r="M8" s="95"/>
+      <c r="N8" s="96"/>
       <c r="O8" s="7"/>
     </row>
     <row r="9" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2288,27 +2294,27 @@
     </row>
     <row r="11" spans="2:16" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B11" s="15"/>
-      <c r="C11" s="121"/>
-      <c r="D11" s="122"/>
-      <c r="E11" s="122"/>
-      <c r="F11" s="144" t="s">
+      <c r="C11" s="122"/>
+      <c r="D11" s="123"/>
+      <c r="E11" s="123"/>
+      <c r="F11" s="145" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="144"/>
-      <c r="H11" s="144"/>
-      <c r="I11" s="144"/>
-      <c r="J11" s="144"/>
-      <c r="K11" s="144"/>
-      <c r="L11" s="144"/>
-      <c r="M11" s="144"/>
-      <c r="N11" s="145"/>
+      <c r="G11" s="145"/>
+      <c r="H11" s="145"/>
+      <c r="I11" s="145"/>
+      <c r="J11" s="145"/>
+      <c r="K11" s="145"/>
+      <c r="L11" s="145"/>
+      <c r="M11" s="145"/>
+      <c r="N11" s="146"/>
       <c r="O11" s="7"/>
     </row>
     <row r="12" spans="2:16" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="14"/>
-      <c r="C12" s="151"/>
-      <c r="D12" s="152"/>
-      <c r="E12" s="152"/>
+      <c r="C12" s="152"/>
+      <c r="D12" s="153"/>
+      <c r="E12" s="153"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
@@ -2322,20 +2328,20 @@
     </row>
     <row r="13" spans="2:16" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="15"/>
-      <c r="C13" s="135" t="s">
+      <c r="C13" s="136" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="136"/>
-      <c r="E13" s="136"/>
-      <c r="F13" s="136"/>
-      <c r="G13" s="136"/>
-      <c r="H13" s="136"/>
-      <c r="I13" s="136"/>
-      <c r="J13" s="136"/>
-      <c r="K13" s="136"/>
-      <c r="L13" s="136"/>
-      <c r="M13" s="136"/>
-      <c r="N13" s="137"/>
+      <c r="D13" s="137"/>
+      <c r="E13" s="137"/>
+      <c r="F13" s="137"/>
+      <c r="G13" s="137"/>
+      <c r="H13" s="137"/>
+      <c r="I13" s="137"/>
+      <c r="J13" s="137"/>
+      <c r="K13" s="137"/>
+      <c r="L13" s="137"/>
+      <c r="M13" s="137"/>
+      <c r="N13" s="138"/>
       <c r="O13" s="7"/>
     </row>
     <row r="14" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2343,23 +2349,23 @@
       <c r="C14" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="154" t="s">
+      <c r="D14" s="155" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="154"/>
-      <c r="F14" s="154"/>
-      <c r="G14" s="154"/>
-      <c r="H14" s="154"/>
-      <c r="I14" s="154"/>
-      <c r="J14" s="155"/>
-      <c r="K14" s="153" t="s">
+      <c r="E14" s="155"/>
+      <c r="F14" s="155"/>
+      <c r="G14" s="155"/>
+      <c r="H14" s="155"/>
+      <c r="I14" s="155"/>
+      <c r="J14" s="156"/>
+      <c r="K14" s="154" t="s">
         <v>9</v>
       </c>
-      <c r="L14" s="153"/>
-      <c r="M14" s="146" t="s">
+      <c r="L14" s="154"/>
+      <c r="M14" s="147" t="s">
         <v>30</v>
       </c>
-      <c r="N14" s="147"/>
+      <c r="N14" s="148"/>
       <c r="O14" s="7"/>
     </row>
     <row r="15" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2367,23 +2373,23 @@
       <c r="C15" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="156" t="s">
+      <c r="D15" s="157" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="156"/>
-      <c r="F15" s="156"/>
-      <c r="G15" s="156"/>
-      <c r="H15" s="156"/>
-      <c r="I15" s="156"/>
-      <c r="J15" s="64" t="s">
+      <c r="E15" s="157"/>
+      <c r="F15" s="157"/>
+      <c r="G15" s="157"/>
+      <c r="H15" s="157"/>
+      <c r="I15" s="157"/>
+      <c r="J15" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="K15" s="64"/>
-      <c r="L15" s="64"/>
-      <c r="M15" s="62" t="s">
+      <c r="K15" s="65"/>
+      <c r="L15" s="65"/>
+      <c r="M15" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="N15" s="63"/>
+      <c r="N15" s="64"/>
       <c r="O15" s="59"/>
     </row>
     <row r="16" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2391,19 +2397,19 @@
       <c r="C16" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="132" t="s">
+      <c r="D16" s="133" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="133"/>
-      <c r="F16" s="133"/>
-      <c r="G16" s="133"/>
-      <c r="H16" s="133"/>
-      <c r="I16" s="133"/>
-      <c r="J16" s="133"/>
-      <c r="K16" s="133"/>
-      <c r="L16" s="133"/>
-      <c r="M16" s="133"/>
-      <c r="N16" s="134"/>
+      <c r="E16" s="134"/>
+      <c r="F16" s="134"/>
+      <c r="G16" s="134"/>
+      <c r="H16" s="134"/>
+      <c r="I16" s="134"/>
+      <c r="J16" s="134"/>
+      <c r="K16" s="134"/>
+      <c r="L16" s="134"/>
+      <c r="M16" s="134"/>
+      <c r="N16" s="135"/>
       <c r="O16" s="7"/>
     </row>
     <row r="17" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2411,13 +2417,13 @@
       <c r="C17" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="62" t="s">
+      <c r="D17" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="62"/>
-      <c r="F17" s="62"/>
-      <c r="G17" s="62"/>
-      <c r="H17" s="62"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="63"/>
       <c r="O17" s="59"/>
     </row>
     <row r="18" spans="2:15" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2441,17 +2447,17 @@
       <c r="C19" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="140" t="s">
+      <c r="D19" s="141" t="s">
         <v>1</v>
       </c>
-      <c r="E19" s="141"/>
-      <c r="F19" s="141"/>
-      <c r="G19" s="141"/>
-      <c r="H19" s="141"/>
-      <c r="I19" s="141"/>
-      <c r="J19" s="141"/>
-      <c r="K19" s="141"/>
-      <c r="L19" s="142"/>
+      <c r="E19" s="142"/>
+      <c r="F19" s="142"/>
+      <c r="G19" s="142"/>
+      <c r="H19" s="142"/>
+      <c r="I19" s="142"/>
+      <c r="J19" s="142"/>
+      <c r="K19" s="142"/>
+      <c r="L19" s="143"/>
       <c r="M19" s="32" t="s">
         <v>8</v>
       </c>
@@ -2463,15 +2469,15 @@
     <row r="20" spans="2:15" ht="3.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="14"/>
       <c r="C20" s="39"/>
-      <c r="D20" s="157"/>
-      <c r="E20" s="85"/>
-      <c r="F20" s="85"/>
-      <c r="G20" s="85"/>
-      <c r="H20" s="85"/>
-      <c r="I20" s="85"/>
-      <c r="J20" s="85"/>
-      <c r="K20" s="85"/>
-      <c r="L20" s="86"/>
+      <c r="D20" s="158"/>
+      <c r="E20" s="86"/>
+      <c r="F20" s="86"/>
+      <c r="G20" s="86"/>
+      <c r="H20" s="86"/>
+      <c r="I20" s="86"/>
+      <c r="J20" s="86"/>
+      <c r="K20" s="86"/>
+      <c r="L20" s="87"/>
       <c r="M20" s="37"/>
       <c r="N20" s="38"/>
       <c r="O20" s="7"/>
@@ -2479,15 +2485,15 @@
     <row r="21" spans="2:15" ht="52.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="14"/>
       <c r="C21" s="39"/>
-      <c r="D21" s="84"/>
-      <c r="E21" s="85"/>
-      <c r="F21" s="85"/>
-      <c r="G21" s="85"/>
-      <c r="H21" s="85"/>
-      <c r="I21" s="85"/>
-      <c r="J21" s="85"/>
-      <c r="K21" s="85"/>
-      <c r="L21" s="86"/>
+      <c r="D21" s="85"/>
+      <c r="E21" s="86"/>
+      <c r="F21" s="86"/>
+      <c r="G21" s="86"/>
+      <c r="H21" s="86"/>
+      <c r="I21" s="86"/>
+      <c r="J21" s="86"/>
+      <c r="K21" s="86"/>
+      <c r="L21" s="87"/>
       <c r="M21" s="37"/>
       <c r="N21" s="38"/>
       <c r="O21" s="7"/>
@@ -2495,15 +2501,15 @@
     <row r="22" spans="2:15" ht="0.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="14"/>
       <c r="C22" s="16"/>
-      <c r="D22" s="72"/>
-      <c r="E22" s="73"/>
-      <c r="F22" s="73"/>
-      <c r="G22" s="73"/>
-      <c r="H22" s="73"/>
-      <c r="I22" s="73"/>
-      <c r="J22" s="73"/>
-      <c r="K22" s="73"/>
-      <c r="L22" s="74"/>
+      <c r="D22" s="73"/>
+      <c r="E22" s="74"/>
+      <c r="F22" s="74"/>
+      <c r="G22" s="74"/>
+      <c r="H22" s="74"/>
+      <c r="I22" s="74"/>
+      <c r="J22" s="74"/>
+      <c r="K22" s="74"/>
+      <c r="L22" s="75"/>
       <c r="M22" s="17"/>
       <c r="N22" s="18"/>
       <c r="O22" s="7"/>
@@ -2511,15 +2517,15 @@
     <row r="23" spans="2:15" ht="0.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="14"/>
       <c r="C23" s="16"/>
-      <c r="D23" s="72"/>
-      <c r="E23" s="73"/>
-      <c r="F23" s="73"/>
-      <c r="G23" s="73"/>
-      <c r="H23" s="73"/>
-      <c r="I23" s="73"/>
-      <c r="J23" s="73"/>
-      <c r="K23" s="73"/>
-      <c r="L23" s="74"/>
+      <c r="D23" s="73"/>
+      <c r="E23" s="74"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="74"/>
+      <c r="H23" s="74"/>
+      <c r="I23" s="74"/>
+      <c r="J23" s="74"/>
+      <c r="K23" s="74"/>
+      <c r="L23" s="75"/>
       <c r="M23" s="17"/>
       <c r="N23" s="18"/>
       <c r="O23" s="7"/>
@@ -2527,15 +2533,15 @@
     <row r="24" spans="2:15" ht="29.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="14"/>
       <c r="C24" s="16"/>
-      <c r="D24" s="72"/>
-      <c r="E24" s="73"/>
-      <c r="F24" s="73"/>
-      <c r="G24" s="73"/>
-      <c r="H24" s="73"/>
-      <c r="I24" s="73"/>
-      <c r="J24" s="73"/>
-      <c r="K24" s="73"/>
-      <c r="L24" s="74"/>
+      <c r="D24" s="73"/>
+      <c r="E24" s="74"/>
+      <c r="F24" s="74"/>
+      <c r="G24" s="74"/>
+      <c r="H24" s="74"/>
+      <c r="I24" s="74"/>
+      <c r="J24" s="74"/>
+      <c r="K24" s="74"/>
+      <c r="L24" s="75"/>
       <c r="M24" s="17"/>
       <c r="N24" s="18"/>
       <c r="O24" s="7"/>
@@ -2543,15 +2549,15 @@
     <row r="25" spans="2:15" ht="42" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" s="14"/>
       <c r="C25" s="16"/>
-      <c r="D25" s="72"/>
-      <c r="E25" s="73"/>
-      <c r="F25" s="73"/>
-      <c r="G25" s="73"/>
-      <c r="H25" s="73"/>
-      <c r="I25" s="73"/>
-      <c r="J25" s="73"/>
-      <c r="K25" s="73"/>
-      <c r="L25" s="74"/>
+      <c r="D25" s="73"/>
+      <c r="E25" s="74"/>
+      <c r="F25" s="74"/>
+      <c r="G25" s="74"/>
+      <c r="H25" s="74"/>
+      <c r="I25" s="74"/>
+      <c r="J25" s="74"/>
+      <c r="K25" s="74"/>
+      <c r="L25" s="75"/>
       <c r="M25" s="17"/>
       <c r="N25" s="18"/>
       <c r="O25" s="7"/>
@@ -2559,15 +2565,15 @@
     <row r="26" spans="2:15" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="14"/>
       <c r="C26" s="16"/>
-      <c r="D26" s="72"/>
-      <c r="E26" s="73"/>
-      <c r="F26" s="73"/>
-      <c r="G26" s="73"/>
-      <c r="H26" s="73"/>
-      <c r="I26" s="73"/>
-      <c r="J26" s="73"/>
-      <c r="K26" s="73"/>
-      <c r="L26" s="74"/>
+      <c r="D26" s="73"/>
+      <c r="E26" s="74"/>
+      <c r="F26" s="74"/>
+      <c r="G26" s="74"/>
+      <c r="H26" s="74"/>
+      <c r="I26" s="74"/>
+      <c r="J26" s="74"/>
+      <c r="K26" s="74"/>
+      <c r="L26" s="75"/>
       <c r="M26" s="17"/>
       <c r="N26" s="18"/>
       <c r="O26" s="7"/>
@@ -2575,15 +2581,15 @@
     <row r="27" spans="2:15" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="14"/>
       <c r="C27" s="16"/>
-      <c r="D27" s="72"/>
-      <c r="E27" s="73"/>
-      <c r="F27" s="73"/>
-      <c r="G27" s="73"/>
-      <c r="H27" s="73"/>
-      <c r="I27" s="73"/>
-      <c r="J27" s="73"/>
-      <c r="K27" s="73"/>
-      <c r="L27" s="74"/>
+      <c r="D27" s="73"/>
+      <c r="E27" s="74"/>
+      <c r="F27" s="74"/>
+      <c r="G27" s="74"/>
+      <c r="H27" s="74"/>
+      <c r="I27" s="74"/>
+      <c r="J27" s="74"/>
+      <c r="K27" s="74"/>
+      <c r="L27" s="75"/>
       <c r="M27" s="17"/>
       <c r="N27" s="18"/>
       <c r="O27" s="7"/>
@@ -2591,15 +2597,15 @@
     <row r="28" spans="2:15" ht="0.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B28" s="14"/>
       <c r="C28" s="16"/>
-      <c r="D28" s="72"/>
-      <c r="E28" s="73"/>
-      <c r="F28" s="73"/>
-      <c r="G28" s="73"/>
-      <c r="H28" s="73"/>
-      <c r="I28" s="73"/>
-      <c r="J28" s="73"/>
-      <c r="K28" s="73"/>
-      <c r="L28" s="74"/>
+      <c r="D28" s="73"/>
+      <c r="E28" s="74"/>
+      <c r="F28" s="74"/>
+      <c r="G28" s="74"/>
+      <c r="H28" s="74"/>
+      <c r="I28" s="74"/>
+      <c r="J28" s="74"/>
+      <c r="K28" s="74"/>
+      <c r="L28" s="75"/>
       <c r="M28" s="17"/>
       <c r="N28" s="18"/>
       <c r="O28" s="7"/>
@@ -2607,15 +2613,15 @@
     <row r="29" spans="2:15" ht="39" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B29" s="14"/>
       <c r="C29" s="16"/>
-      <c r="D29" s="72"/>
-      <c r="E29" s="73"/>
-      <c r="F29" s="73"/>
-      <c r="G29" s="73"/>
-      <c r="H29" s="73"/>
-      <c r="I29" s="73"/>
-      <c r="J29" s="73"/>
-      <c r="K29" s="73"/>
-      <c r="L29" s="74"/>
+      <c r="D29" s="73"/>
+      <c r="E29" s="74"/>
+      <c r="F29" s="74"/>
+      <c r="G29" s="74"/>
+      <c r="H29" s="74"/>
+      <c r="I29" s="74"/>
+      <c r="J29" s="74"/>
+      <c r="K29" s="74"/>
+      <c r="L29" s="75"/>
       <c r="M29" s="17"/>
       <c r="N29" s="18"/>
       <c r="O29" s="7"/>
@@ -2623,15 +2629,15 @@
     <row r="30" spans="2:15" ht="39" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="14"/>
       <c r="C30" s="16"/>
-      <c r="D30" s="72"/>
-      <c r="E30" s="73"/>
-      <c r="F30" s="73"/>
-      <c r="G30" s="73"/>
-      <c r="H30" s="73"/>
-      <c r="I30" s="73"/>
-      <c r="J30" s="73"/>
-      <c r="K30" s="73"/>
-      <c r="L30" s="74"/>
+      <c r="D30" s="73"/>
+      <c r="E30" s="74"/>
+      <c r="F30" s="74"/>
+      <c r="G30" s="74"/>
+      <c r="H30" s="74"/>
+      <c r="I30" s="74"/>
+      <c r="J30" s="74"/>
+      <c r="K30" s="74"/>
+      <c r="L30" s="75"/>
       <c r="M30" s="17"/>
       <c r="N30" s="18"/>
       <c r="O30" s="7"/>
@@ -2639,15 +2645,15 @@
     <row r="31" spans="2:15" ht="39" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B31" s="14"/>
       <c r="C31" s="16"/>
-      <c r="D31" s="72"/>
-      <c r="E31" s="73"/>
-      <c r="F31" s="73"/>
-      <c r="G31" s="73"/>
-      <c r="H31" s="73"/>
-      <c r="I31" s="73"/>
-      <c r="J31" s="73"/>
-      <c r="K31" s="73"/>
-      <c r="L31" s="74"/>
+      <c r="D31" s="73"/>
+      <c r="E31" s="74"/>
+      <c r="F31" s="74"/>
+      <c r="G31" s="74"/>
+      <c r="H31" s="74"/>
+      <c r="I31" s="74"/>
+      <c r="J31" s="74"/>
+      <c r="K31" s="74"/>
+      <c r="L31" s="75"/>
       <c r="M31" s="17"/>
       <c r="N31" s="18"/>
       <c r="O31" s="7"/>
@@ -2655,15 +2661,15 @@
     <row r="32" spans="2:15" ht="39" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B32" s="14"/>
       <c r="C32" s="16"/>
-      <c r="D32" s="72"/>
-      <c r="E32" s="73"/>
-      <c r="F32" s="73"/>
-      <c r="G32" s="73"/>
-      <c r="H32" s="73"/>
-      <c r="I32" s="73"/>
-      <c r="J32" s="73"/>
-      <c r="K32" s="73"/>
-      <c r="L32" s="74"/>
+      <c r="D32" s="73"/>
+      <c r="E32" s="74"/>
+      <c r="F32" s="74"/>
+      <c r="G32" s="74"/>
+      <c r="H32" s="74"/>
+      <c r="I32" s="74"/>
+      <c r="J32" s="74"/>
+      <c r="K32" s="74"/>
+      <c r="L32" s="75"/>
       <c r="M32" s="17"/>
       <c r="N32" s="18"/>
       <c r="O32" s="7"/>
@@ -2671,15 +2677,15 @@
     <row r="33" spans="2:15" ht="39" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="14"/>
       <c r="C33" s="16"/>
-      <c r="D33" s="72"/>
-      <c r="E33" s="73"/>
-      <c r="F33" s="73"/>
-      <c r="G33" s="73"/>
-      <c r="H33" s="73"/>
-      <c r="I33" s="73"/>
-      <c r="J33" s="73"/>
-      <c r="K33" s="73"/>
-      <c r="L33" s="74"/>
+      <c r="D33" s="73"/>
+      <c r="E33" s="74"/>
+      <c r="F33" s="74"/>
+      <c r="G33" s="74"/>
+      <c r="H33" s="74"/>
+      <c r="I33" s="74"/>
+      <c r="J33" s="74"/>
+      <c r="K33" s="74"/>
+      <c r="L33" s="75"/>
       <c r="M33" s="17"/>
       <c r="N33" s="18"/>
       <c r="O33" s="7"/>
@@ -2687,15 +2693,15 @@
     <row r="34" spans="2:15" ht="39" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="14"/>
       <c r="C34" s="16"/>
-      <c r="D34" s="72"/>
-      <c r="E34" s="73"/>
-      <c r="F34" s="73"/>
-      <c r="G34" s="73"/>
-      <c r="H34" s="73"/>
-      <c r="I34" s="73"/>
-      <c r="J34" s="73"/>
-      <c r="K34" s="73"/>
-      <c r="L34" s="74"/>
+      <c r="D34" s="73"/>
+      <c r="E34" s="74"/>
+      <c r="F34" s="74"/>
+      <c r="G34" s="74"/>
+      <c r="H34" s="74"/>
+      <c r="I34" s="74"/>
+      <c r="J34" s="74"/>
+      <c r="K34" s="74"/>
+      <c r="L34" s="75"/>
       <c r="M34" s="17"/>
       <c r="N34" s="18"/>
       <c r="O34" s="7"/>
@@ -2703,15 +2709,15 @@
     <row r="35" spans="2:15" ht="39" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="14"/>
       <c r="C35" s="16"/>
-      <c r="D35" s="72"/>
-      <c r="E35" s="73"/>
-      <c r="F35" s="73"/>
-      <c r="G35" s="73"/>
-      <c r="H35" s="73"/>
-      <c r="I35" s="73"/>
-      <c r="J35" s="73"/>
-      <c r="K35" s="73"/>
-      <c r="L35" s="74"/>
+      <c r="D35" s="73"/>
+      <c r="E35" s="74"/>
+      <c r="F35" s="74"/>
+      <c r="G35" s="74"/>
+      <c r="H35" s="74"/>
+      <c r="I35" s="74"/>
+      <c r="J35" s="74"/>
+      <c r="K35" s="74"/>
+      <c r="L35" s="75"/>
       <c r="M35" s="17"/>
       <c r="N35" s="18"/>
       <c r="O35" s="7"/>
@@ -2719,15 +2725,15 @@
     <row r="36" spans="2:15" ht="39" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="14"/>
       <c r="C36" s="16"/>
-      <c r="D36" s="72"/>
-      <c r="E36" s="73"/>
-      <c r="F36" s="73"/>
-      <c r="G36" s="73"/>
-      <c r="H36" s="73"/>
-      <c r="I36" s="73"/>
-      <c r="J36" s="73"/>
-      <c r="K36" s="73"/>
-      <c r="L36" s="74"/>
+      <c r="D36" s="73"/>
+      <c r="E36" s="74"/>
+      <c r="F36" s="74"/>
+      <c r="G36" s="74"/>
+      <c r="H36" s="74"/>
+      <c r="I36" s="74"/>
+      <c r="J36" s="74"/>
+      <c r="K36" s="74"/>
+      <c r="L36" s="75"/>
       <c r="M36" s="17"/>
       <c r="N36" s="18"/>
       <c r="O36" s="7"/>
@@ -2735,15 +2741,15 @@
     <row r="37" spans="2:15" ht="39" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="14"/>
       <c r="C37" s="16"/>
-      <c r="D37" s="72"/>
-      <c r="E37" s="73"/>
-      <c r="F37" s="73"/>
-      <c r="G37" s="73"/>
-      <c r="H37" s="73"/>
-      <c r="I37" s="73"/>
-      <c r="J37" s="73"/>
-      <c r="K37" s="73"/>
-      <c r="L37" s="74"/>
+      <c r="D37" s="73"/>
+      <c r="E37" s="74"/>
+      <c r="F37" s="74"/>
+      <c r="G37" s="74"/>
+      <c r="H37" s="74"/>
+      <c r="I37" s="74"/>
+      <c r="J37" s="74"/>
+      <c r="K37" s="74"/>
+      <c r="L37" s="75"/>
       <c r="M37" s="17"/>
       <c r="N37" s="18"/>
       <c r="O37" s="7"/>
@@ -2751,15 +2757,15 @@
     <row r="38" spans="2:15" ht="39" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="14"/>
       <c r="C38" s="16"/>
-      <c r="D38" s="72"/>
-      <c r="E38" s="73"/>
-      <c r="F38" s="73"/>
-      <c r="G38" s="73"/>
-      <c r="H38" s="73"/>
-      <c r="I38" s="73"/>
-      <c r="J38" s="73"/>
-      <c r="K38" s="73"/>
-      <c r="L38" s="74"/>
+      <c r="D38" s="73"/>
+      <c r="E38" s="74"/>
+      <c r="F38" s="74"/>
+      <c r="G38" s="74"/>
+      <c r="H38" s="74"/>
+      <c r="I38" s="74"/>
+      <c r="J38" s="74"/>
+      <c r="K38" s="74"/>
+      <c r="L38" s="75"/>
       <c r="M38" s="17"/>
       <c r="N38" s="18"/>
       <c r="O38" s="7"/>
@@ -2767,15 +2773,15 @@
     <row r="39" spans="2:15" ht="39" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="14"/>
       <c r="C39" s="16"/>
-      <c r="D39" s="72"/>
-      <c r="E39" s="73"/>
-      <c r="F39" s="73"/>
-      <c r="G39" s="73"/>
-      <c r="H39" s="73"/>
-      <c r="I39" s="73"/>
-      <c r="J39" s="73"/>
-      <c r="K39" s="73"/>
-      <c r="L39" s="74"/>
+      <c r="D39" s="73"/>
+      <c r="E39" s="74"/>
+      <c r="F39" s="74"/>
+      <c r="G39" s="74"/>
+      <c r="H39" s="74"/>
+      <c r="I39" s="74"/>
+      <c r="J39" s="74"/>
+      <c r="K39" s="74"/>
+      <c r="L39" s="75"/>
       <c r="M39" s="17"/>
       <c r="N39" s="18"/>
       <c r="O39" s="7"/>
@@ -2783,15 +2789,15 @@
     <row r="40" spans="2:15" ht="39" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="14"/>
       <c r="C40" s="16"/>
-      <c r="D40" s="72"/>
-      <c r="E40" s="73"/>
-      <c r="F40" s="73"/>
-      <c r="G40" s="73"/>
-      <c r="H40" s="73"/>
-      <c r="I40" s="73"/>
-      <c r="J40" s="73"/>
-      <c r="K40" s="73"/>
-      <c r="L40" s="74"/>
+      <c r="D40" s="73"/>
+      <c r="E40" s="74"/>
+      <c r="F40" s="74"/>
+      <c r="G40" s="74"/>
+      <c r="H40" s="74"/>
+      <c r="I40" s="74"/>
+      <c r="J40" s="74"/>
+      <c r="K40" s="74"/>
+      <c r="L40" s="75"/>
       <c r="M40" s="17"/>
       <c r="N40" s="18"/>
       <c r="O40" s="7"/>
@@ -2799,15 +2805,15 @@
     <row r="41" spans="2:15" ht="39" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="14"/>
       <c r="C41" s="16"/>
-      <c r="D41" s="72"/>
-      <c r="E41" s="73"/>
-      <c r="F41" s="73"/>
-      <c r="G41" s="73"/>
-      <c r="H41" s="73"/>
-      <c r="I41" s="73"/>
-      <c r="J41" s="73"/>
-      <c r="K41" s="73"/>
-      <c r="L41" s="74"/>
+      <c r="D41" s="73"/>
+      <c r="E41" s="74"/>
+      <c r="F41" s="74"/>
+      <c r="G41" s="74"/>
+      <c r="H41" s="74"/>
+      <c r="I41" s="74"/>
+      <c r="J41" s="74"/>
+      <c r="K41" s="74"/>
+      <c r="L41" s="75"/>
       <c r="M41" s="17"/>
       <c r="N41" s="18"/>
       <c r="O41" s="7"/>
@@ -2815,15 +2821,15 @@
     <row r="42" spans="2:15" ht="75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="14"/>
       <c r="C42" s="16"/>
-      <c r="D42" s="100"/>
-      <c r="E42" s="101"/>
-      <c r="F42" s="101"/>
-      <c r="G42" s="101"/>
-      <c r="H42" s="101"/>
-      <c r="I42" s="101"/>
-      <c r="J42" s="101"/>
-      <c r="K42" s="101"/>
-      <c r="L42" s="102"/>
+      <c r="D42" s="101"/>
+      <c r="E42" s="102"/>
+      <c r="F42" s="102"/>
+      <c r="G42" s="102"/>
+      <c r="H42" s="102"/>
+      <c r="I42" s="102"/>
+      <c r="J42" s="102"/>
+      <c r="K42" s="102"/>
+      <c r="L42" s="103"/>
       <c r="M42" s="17"/>
       <c r="N42" s="18"/>
       <c r="O42" s="7"/>
@@ -2833,15 +2839,15 @@
       <c r="C43" s="16">
         <v>1</v>
       </c>
-      <c r="D43" s="106"/>
-      <c r="E43" s="126"/>
-      <c r="F43" s="126"/>
-      <c r="G43" s="126"/>
-      <c r="H43" s="126"/>
-      <c r="I43" s="126"/>
-      <c r="J43" s="126"/>
-      <c r="K43" s="126"/>
-      <c r="L43" s="127"/>
+      <c r="D43" s="107"/>
+      <c r="E43" s="127"/>
+      <c r="F43" s="127"/>
+      <c r="G43" s="127"/>
+      <c r="H43" s="127"/>
+      <c r="I43" s="127"/>
+      <c r="J43" s="127"/>
+      <c r="K43" s="127"/>
+      <c r="L43" s="128"/>
       <c r="M43" s="61" t="s">
         <v>25</v>
       </c>
@@ -2853,33 +2859,33 @@
     <row r="44" spans="2:15" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="14"/>
       <c r="C44" s="16"/>
-      <c r="D44" s="106"/>
-      <c r="E44" s="107"/>
-      <c r="F44" s="107"/>
-      <c r="G44" s="107"/>
-      <c r="H44" s="107"/>
-      <c r="I44" s="107"/>
-      <c r="J44" s="107"/>
-      <c r="K44" s="107"/>
-      <c r="L44" s="108"/>
-      <c r="M44" s="17"/>
-      <c r="N44" s="18"/>
+      <c r="D44" s="107"/>
+      <c r="E44" s="108"/>
+      <c r="F44" s="108"/>
+      <c r="G44" s="108"/>
+      <c r="H44" s="108"/>
+      <c r="I44" s="108"/>
+      <c r="J44" s="108"/>
+      <c r="K44" s="108"/>
+      <c r="L44" s="109"/>
+      <c r="M44" s="61"/>
+      <c r="N44" s="62"/>
       <c r="O44" s="7"/>
     </row>
     <row r="45" spans="2:15" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="14"/>
       <c r="C45" s="16"/>
-      <c r="D45" s="123" t="s">
+      <c r="D45" s="124" t="s">
         <v>24</v>
       </c>
-      <c r="E45" s="124"/>
-      <c r="F45" s="124"/>
-      <c r="G45" s="124"/>
-      <c r="H45" s="124"/>
-      <c r="I45" s="124"/>
-      <c r="J45" s="124"/>
-      <c r="K45" s="124"/>
-      <c r="L45" s="125"/>
+      <c r="E45" s="125"/>
+      <c r="F45" s="125"/>
+      <c r="G45" s="125"/>
+      <c r="H45" s="125"/>
+      <c r="I45" s="125"/>
+      <c r="J45" s="125"/>
+      <c r="K45" s="125"/>
+      <c r="L45" s="126"/>
       <c r="M45" s="17"/>
       <c r="N45" s="18"/>
       <c r="O45" s="7"/>
@@ -2887,48 +2893,48 @@
     <row r="46" spans="2:15" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="14"/>
       <c r="C46" s="16"/>
-      <c r="D46" s="81" t="s">
+      <c r="D46" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="E46" s="82"/>
-      <c r="F46" s="82"/>
-      <c r="G46" s="82"/>
-      <c r="H46" s="82"/>
-      <c r="I46" s="82"/>
-      <c r="J46" s="82"/>
-      <c r="K46" s="82"/>
-      <c r="L46" s="83"/>
+      <c r="E46" s="83"/>
+      <c r="F46" s="83"/>
+      <c r="G46" s="83"/>
+      <c r="H46" s="83"/>
+      <c r="I46" s="83"/>
+      <c r="J46" s="83"/>
+      <c r="K46" s="83"/>
+      <c r="L46" s="84"/>
       <c r="M46" s="17"/>
       <c r="N46" s="18"/>
       <c r="O46" s="7"/>
     </row>
     <row r="47" spans="2:15" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B47" s="14"/>
-      <c r="C47" s="148"/>
-      <c r="D47" s="149"/>
-      <c r="E47" s="149"/>
-      <c r="F47" s="149"/>
-      <c r="G47" s="149"/>
-      <c r="H47" s="149"/>
-      <c r="I47" s="150"/>
-      <c r="J47" s="98" t="s">
+      <c r="C47" s="149"/>
+      <c r="D47" s="150"/>
+      <c r="E47" s="150"/>
+      <c r="F47" s="150"/>
+      <c r="G47" s="150"/>
+      <c r="H47" s="150"/>
+      <c r="I47" s="151"/>
+      <c r="J47" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="K47" s="99"/>
-      <c r="L47" s="99"/>
-      <c r="M47" s="138" t="s">
-        <v>25</v>
-      </c>
-      <c r="N47" s="139"/>
+      <c r="K47" s="100"/>
+      <c r="L47" s="100"/>
+      <c r="M47" s="139" t="s">
+        <v>35</v>
+      </c>
+      <c r="N47" s="140"/>
       <c r="O47" s="7"/>
     </row>
     <row r="48" spans="2:15" ht="1.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B48" s="14"/>
-      <c r="C48" s="143"/>
-      <c r="D48" s="143"/>
-      <c r="E48" s="143"/>
-      <c r="F48" s="80"/>
-      <c r="G48" s="80"/>
+      <c r="C48" s="144"/>
+      <c r="D48" s="144"/>
+      <c r="E48" s="144"/>
+      <c r="F48" s="81"/>
+      <c r="G48" s="81"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
@@ -2940,126 +2946,126 @@
     </row>
     <row r="49" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="14"/>
-      <c r="C49" s="129"/>
-      <c r="D49" s="130"/>
-      <c r="E49" s="130"/>
-      <c r="F49" s="130"/>
-      <c r="G49" s="130"/>
-      <c r="H49" s="130"/>
-      <c r="I49" s="130"/>
-      <c r="J49" s="130"/>
-      <c r="K49" s="130"/>
-      <c r="L49" s="130"/>
-      <c r="M49" s="130"/>
-      <c r="N49" s="131"/>
+      <c r="C49" s="130"/>
+      <c r="D49" s="131"/>
+      <c r="E49" s="131"/>
+      <c r="F49" s="131"/>
+      <c r="G49" s="131"/>
+      <c r="H49" s="131"/>
+      <c r="I49" s="131"/>
+      <c r="J49" s="131"/>
+      <c r="K49" s="131"/>
+      <c r="L49" s="131"/>
+      <c r="M49" s="131"/>
+      <c r="N49" s="132"/>
       <c r="O49" s="7"/>
     </row>
     <row r="50" spans="2:15" s="22" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="21"/>
-      <c r="C50" s="116" t="s">
+      <c r="C50" s="117" t="s">
         <v>33</v>
       </c>
-      <c r="D50" s="117"/>
+      <c r="D50" s="118"/>
       <c r="E50" s="40"/>
       <c r="F50" s="40"/>
       <c r="G50" s="40"/>
-      <c r="H50" s="113" t="s">
+      <c r="H50" s="114" t="s">
         <v>34</v>
       </c>
-      <c r="I50" s="114"/>
-      <c r="J50" s="114"/>
-      <c r="K50" s="114"/>
-      <c r="L50" s="114"/>
-      <c r="M50" s="114"/>
-      <c r="N50" s="115"/>
+      <c r="I50" s="115"/>
+      <c r="J50" s="115"/>
+      <c r="K50" s="115"/>
+      <c r="L50" s="115"/>
+      <c r="M50" s="115"/>
+      <c r="N50" s="116"/>
       <c r="O50" s="7"/>
     </row>
     <row r="51" spans="2:15" s="22" customFormat="1" ht="0.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="21"/>
-      <c r="C51" s="110"/>
-      <c r="D51" s="111"/>
-      <c r="E51" s="111"/>
-      <c r="F51" s="111"/>
-      <c r="G51" s="111"/>
-      <c r="H51" s="111"/>
-      <c r="I51" s="111"/>
-      <c r="J51" s="111"/>
-      <c r="K51" s="111"/>
-      <c r="L51" s="111"/>
-      <c r="M51" s="111"/>
-      <c r="N51" s="112"/>
+      <c r="C51" s="111"/>
+      <c r="D51" s="112"/>
+      <c r="E51" s="112"/>
+      <c r="F51" s="112"/>
+      <c r="G51" s="112"/>
+      <c r="H51" s="112"/>
+      <c r="I51" s="112"/>
+      <c r="J51" s="112"/>
+      <c r="K51" s="112"/>
+      <c r="L51" s="112"/>
+      <c r="M51" s="112"/>
+      <c r="N51" s="113"/>
       <c r="O51" s="7"/>
     </row>
     <row r="52" spans="2:15" s="22" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="21"/>
-      <c r="C52" s="90" t="s">
+      <c r="C52" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="D52" s="91"/>
-      <c r="E52" s="119"/>
-      <c r="F52" s="119"/>
+      <c r="D52" s="92"/>
+      <c r="E52" s="120"/>
+      <c r="F52" s="120"/>
       <c r="G52" s="41"/>
-      <c r="H52" s="88" t="s">
+      <c r="H52" s="89" t="s">
         <v>32</v>
       </c>
-      <c r="I52" s="88"/>
-      <c r="J52" s="88"/>
-      <c r="K52" s="88"/>
-      <c r="L52" s="88"/>
-      <c r="M52" s="88"/>
-      <c r="N52" s="89"/>
+      <c r="I52" s="89"/>
+      <c r="J52" s="89"/>
+      <c r="K52" s="89"/>
+      <c r="L52" s="89"/>
+      <c r="M52" s="89"/>
+      <c r="N52" s="90"/>
       <c r="O52" s="7"/>
     </row>
     <row r="53" spans="2:15" s="22" customFormat="1" ht="21" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B53" s="21"/>
-      <c r="C53" s="118"/>
+      <c r="C53" s="119"/>
       <c r="D53" s="42"/>
       <c r="E53" s="43"/>
       <c r="F53" s="43"/>
       <c r="G53" s="43"/>
-      <c r="H53" s="75"/>
-      <c r="I53" s="76"/>
-      <c r="J53" s="87"/>
-      <c r="K53" s="87"/>
-      <c r="L53" s="87"/>
-      <c r="M53" s="75"/>
-      <c r="N53" s="105"/>
+      <c r="H53" s="76"/>
+      <c r="I53" s="77"/>
+      <c r="J53" s="88"/>
+      <c r="K53" s="88"/>
+      <c r="L53" s="88"/>
+      <c r="M53" s="76"/>
+      <c r="N53" s="106"/>
       <c r="O53" s="7"/>
     </row>
     <row r="54" spans="2:15" s="22" customFormat="1" ht="21" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B54" s="21"/>
-      <c r="C54" s="118"/>
+      <c r="C54" s="119"/>
       <c r="D54" s="44"/>
       <c r="E54" s="45"/>
       <c r="F54" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="G54" s="70"/>
-      <c r="H54" s="70"/>
-      <c r="I54" s="77"/>
-      <c r="J54" s="68"/>
-      <c r="K54" s="68"/>
-      <c r="L54" s="68"/>
-      <c r="M54" s="70"/>
-      <c r="N54" s="71"/>
+      <c r="G54" s="71"/>
+      <c r="H54" s="71"/>
+      <c r="I54" s="78"/>
+      <c r="J54" s="69"/>
+      <c r="K54" s="69"/>
+      <c r="L54" s="69"/>
+      <c r="M54" s="71"/>
+      <c r="N54" s="72"/>
       <c r="O54" s="7"/>
     </row>
     <row r="55" spans="2:15" s="22" customFormat="1" ht="27.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B55" s="21"/>
-      <c r="C55" s="118"/>
+      <c r="C55" s="119"/>
       <c r="D55" s="47"/>
       <c r="E55" s="48"/>
       <c r="F55" s="49" t="s">
         <v>10</v>
       </c>
       <c r="G55" s="50"/>
-      <c r="H55" s="78"/>
-      <c r="I55" s="79"/>
-      <c r="J55" s="69"/>
-      <c r="K55" s="69"/>
-      <c r="L55" s="69"/>
-      <c r="M55" s="78"/>
-      <c r="N55" s="109"/>
+      <c r="H55" s="79"/>
+      <c r="I55" s="80"/>
+      <c r="J55" s="70"/>
+      <c r="K55" s="70"/>
+      <c r="L55" s="70"/>
+      <c r="M55" s="79"/>
+      <c r="N55" s="110"/>
       <c r="O55" s="7"/>
     </row>
     <row r="56" spans="2:15" s="22" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -3070,30 +3076,30 @@
       <c r="F56" s="52"/>
       <c r="G56" s="52"/>
       <c r="H56" s="52"/>
-      <c r="I56" s="103"/>
-      <c r="J56" s="103"/>
-      <c r="K56" s="103"/>
-      <c r="L56" s="103"/>
-      <c r="M56" s="103"/>
-      <c r="N56" s="104"/>
+      <c r="I56" s="104"/>
+      <c r="J56" s="104"/>
+      <c r="K56" s="104"/>
+      <c r="L56" s="104"/>
+      <c r="M56" s="104"/>
+      <c r="N56" s="105"/>
       <c r="O56" s="7"/>
     </row>
     <row r="57" spans="2:15" s="22" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="21"/>
-      <c r="C57" s="96" t="s">
+      <c r="C57" s="97" t="s">
         <v>21</v>
       </c>
-      <c r="D57" s="97"/>
-      <c r="E57" s="97"/>
-      <c r="F57" s="97"/>
-      <c r="G57" s="97"/>
+      <c r="D57" s="98"/>
+      <c r="E57" s="98"/>
+      <c r="F57" s="98"/>
+      <c r="G57" s="98"/>
       <c r="H57" s="53"/>
       <c r="I57" s="54"/>
-      <c r="J57" s="97"/>
-      <c r="K57" s="97"/>
-      <c r="L57" s="97"/>
-      <c r="M57" s="97"/>
-      <c r="N57" s="120"/>
+      <c r="J57" s="98"/>
+      <c r="K57" s="98"/>
+      <c r="L57" s="98"/>
+      <c r="M57" s="98"/>
+      <c r="N57" s="121"/>
       <c r="O57" s="7"/>
     </row>
     <row r="58" spans="2:15" s="22" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3106,14 +3112,14 @@
       <c r="F58" s="56"/>
       <c r="G58" s="56"/>
       <c r="H58" s="57"/>
-      <c r="I58" s="65" t="s">
+      <c r="I58" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="J58" s="66"/>
-      <c r="K58" s="66"/>
-      <c r="L58" s="66"/>
-      <c r="M58" s="66"/>
-      <c r="N58" s="67"/>
+      <c r="J58" s="67"/>
+      <c r="K58" s="67"/>
+      <c r="L58" s="67"/>
+      <c r="M58" s="67"/>
+      <c r="N58" s="68"/>
       <c r="O58" s="7"/>
     </row>
     <row r="59" spans="2:15" s="22" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">

</xml_diff>